<commit_message>
EPBDS-8958 Comparison operators are not symmetrical for inheritable types (Timestamp vs Date). fixed
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/Comparison_cmp-date.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/Comparison_cmp-date.xlsx
@@ -1,20 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\openL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{819ECF97-1D01-4E06-8049-272EEB8D9897}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="180" windowWidth="27795" windowHeight="12525"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Date" sheetId="14" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="60">
   <si>
     <t>Step</t>
   </si>
@@ -155,13 +169,52 @@
   </si>
   <si>
     <t>= a &lt;&gt; null</t>
+  </si>
+  <si>
+    <t>Test comparisonDate2</t>
+  </si>
+  <si>
+    <t>Environment</t>
+  </si>
+  <si>
+    <t>import</t>
+  </si>
+  <si>
+    <t>2017-10-13</t>
+  </si>
+  <si>
+    <t>2017-10-13 00:00:00</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult comparisonDate3 (Date a, Timestamp b )</t>
+  </si>
+  <si>
+    <t>Test comparisonDate3</t>
+  </si>
+  <si>
+    <t>RETURN</t>
+  </si>
+  <si>
+    <t>java.sql.Timestamp</t>
+  </si>
+  <si>
+    <t>= comparisonDate(a, b)</t>
+  </si>
+  <si>
+    <t>Spreadsheet SpreadsheetResult comparisonDate2 (Timestamp a, Date b )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2017-10-13 00:00:00 </t>
+  </si>
+  <si>
+    <t>when comparing a timestamp with nanoseconds and a date (there are no nanoseconds in the date). behavior differs in java 8 and 11, as in java 8 nanoseconds do not count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -176,8 +229,19 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,8 +254,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="43"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -260,6 +336,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyProtection="0">
@@ -272,7 +357,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -286,6 +371,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="2" xfId="1" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -295,17 +397,20 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="ACT_H" xfId="2"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="ACT_H" xfId="2" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -321,9 +426,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -361,9 +466,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -396,9 +501,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -431,9 +553,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -606,11 +745,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AF34"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A3:AF58"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M55" sqref="M55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -618,9 +757,11 @@
     <col min="1" max="1" width="8.5703125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="2" max="2" width="13.7109375" style="1" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="8.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="7" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="18.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="7" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="7" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="10" width="10.140625" style="1" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="22.42578125" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="10" style="1" customWidth="1" collapsed="1"/>
     <col min="13" max="13" width="17.85546875" style="1" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="14" max="14" width="10" style="1" bestFit="1" customWidth="1" collapsed="1"/>
@@ -935,18 +1076,18 @@
       <c r="P12" s="4"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17"/>
+      <c r="G14" s="17"/>
+      <c r="H14" s="17"/>
+      <c r="I14" s="17"/>
+      <c r="J14" s="17"/>
+      <c r="K14" s="17"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B15" s="7" t="s">
@@ -975,12 +1116,17 @@
       <c r="K15" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="M15" s="9" t="s">
+      <c r="M15" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="11"/>
+      <c r="N15" s="19"/>
+      <c r="O15" s="19"/>
+      <c r="P15" s="20"/>
+      <c r="R15" s="21" t="s">
+        <v>48</v>
+      </c>
+      <c r="S15" s="21"/>
+      <c r="T15" s="21"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
@@ -1019,6 +1165,13 @@
         <v>17</v>
       </c>
       <c r="P16" s="7"/>
+      <c r="R16" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="S16" s="22" t="s">
+        <v>55</v>
+      </c>
+      <c r="T16" s="23"/>
     </row>
     <row r="17" spans="2:16" x14ac:dyDescent="0.2">
       <c r="B17" s="7" t="s">
@@ -1304,66 +1457,308 @@
         <v>1</v>
       </c>
     </row>
+    <row r="26" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="C26" s="3"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+    </row>
     <row r="27" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2"/>
-      <c r="I27" s="2"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
+      <c r="B27" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D27" s="12"/>
+    </row>
+    <row r="28" spans="2:16" x14ac:dyDescent="0.2">
+      <c r="B28" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="5"/>
     </row>
     <row r="29" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="F29" s="5"/>
-      <c r="G29" s="5"/>
-      <c r="H29" s="5"/>
-      <c r="I29" s="5"/>
-      <c r="J29" s="5"/>
-      <c r="K29" s="4"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
     </row>
     <row r="30" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
-      <c r="H30" s="4"/>
-      <c r="I30" s="4"/>
-      <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
+      <c r="B30" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="C30" s="15"/>
+      <c r="D30" s="15"/>
     </row>
     <row r="31" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
+      <c r="B31" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31" s="11" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="32" spans="2:16" x14ac:dyDescent="0.2">
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
-      <c r="H32" s="4"/>
-      <c r="I32" s="4"/>
-      <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-    </row>
-    <row r="33" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
-      <c r="H33" s="4"/>
-      <c r="I33" s="4"/>
-      <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-    </row>
-    <row r="34" spans="6:11" x14ac:dyDescent="0.2">
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
-      <c r="H34" s="4"/>
-      <c r="I34" s="4"/>
-      <c r="J34" s="4"/>
-      <c r="K34" s="4"/>
+      <c r="B32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D33" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D34" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D35" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D36" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D37" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B38" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C38" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D38" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D39" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C42" s="3"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B43" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B44" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="C44" s="13" t="s">
+        <v>56</v>
+      </c>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+    </row>
+    <row r="45" spans="2:6" ht="12" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B45" s="3"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+      <c r="E45" s="4"/>
+      <c r="F45" s="4"/>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B47" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="C47" s="15"/>
+      <c r="D47" s="15"/>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B48" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C48" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D48" s="10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B49" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C49" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B50" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C50" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="D50" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B51" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D51" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B52" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D52" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B53" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C53" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D53" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B54" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C54" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="D54" s="6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B55" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="C55" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D55" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B56" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C56" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D56" s="6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B58" s="1" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="6">
+    <mergeCell ref="B47:D47"/>
+    <mergeCell ref="B30:D30"/>
     <mergeCell ref="B14:K14"/>
     <mergeCell ref="M15:P15"/>
+    <mergeCell ref="R15:T15"/>
+    <mergeCell ref="S16:T16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>